<commit_message>
12.07.2023 End of the Day, M1 Commit after long delay in the dev Working on the AppActions & Club Management
</commit_message>
<xml_diff>
--- a/spec/fs_front_fnctions.xlsx
+++ b/spec/fs_front_fnctions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="PI" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,8 @@
     <sheet name="Main Navi" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Identity" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Club" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="API BackEnd" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Refactor" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="194">
   <si>
     <t xml:space="preserve">PI Nr.</t>
   </si>
@@ -115,6 +117,15 @@
     <t xml:space="preserve">Github Repo</t>
   </si>
   <si>
+    <t xml:space="preserve">12.07.2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AccountManage, AppAction, FSA: club_manager IU, GetClubsRolesActionsResponse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Next: implement actions for browsing club (get basic info, get user list, add / remove user etc)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Root</t>
   </si>
   <si>
@@ -127,321 +138,333 @@
     <t xml:space="preserve">Member</t>
   </si>
   <si>
+    <t xml:space="preserve">Guest</t>
+  </si>
+  <si>
     <t xml:space="preserve">Create Club</t>
   </si>
   <si>
+    <t xml:space="preserve">O</t>
+  </si>
+  <si>
     <t xml:space="preserve">X</t>
   </si>
   <si>
-    <t xml:space="preserve">Change Club Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O</t>
+    <t xml:space="preserve">Read Club Base Info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Club Members List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Club Base Info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Club name, comment, visibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Club Members</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChangeClubPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hand-over Club</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If club has multiple owners, they shall confirm (process TBD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Join Club</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leave Club</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete Club</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assign Owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unassign Owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assign Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unassign Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invite Member</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove Member</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Checklist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Checklist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read Checklist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if visibility setting allows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hand-over Checklist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hand-Over Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Aircraft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Aircraft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read Aircraft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hand-over Aircraft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub-Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complexity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API Ver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Light / Dark Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Splash Screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android 12+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Current Date / Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move to future provider as stream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sig-in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refactor Menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use-case if user is already signed in (user / club)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Font Size in Widgets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch to Theme Style with delta Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Routing to Sign-In</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to Sign-in form in case of 401 response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tab order, skip icon button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skip icon buttons for navigation in form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto Login (credential stored in the App)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plane Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Club Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LogAs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserOrClub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Club</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ListedClub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conditions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AppBar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings Icon Top-Right Corner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bottom Panel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Representation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register New User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API exists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign-in User from Sing-in Form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plain password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign-in User at App Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hashed password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign-in User in On-line mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change User Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password shall not be used by other users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Password Recover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change User Avatar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personal Data Download</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mark user as deleted in DB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Days Impl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sing-in Club from Sign-In Form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">increased</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign-in Club at App Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign-in Club Once switching to On-Line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rename Club</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change Club Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change Club Avatar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A for V4</t>
   </si>
   <si>
     <t xml:space="preserve">Change Club Visibility</t>
   </si>
   <si>
-    <t xml:space="preserve">Hand-over Club</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If club has multiple owners, they shall confirm (process TBD)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leave Club</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete Club</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assign Owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unassign Owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assign Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unassign Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remove Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invite Member</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remove Member</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create Checklist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edit Checklist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read Checklist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if visibility setting allows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hand-over Checklist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edit Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hand-Over Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create Aircraft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edit Aircraft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read Aircraft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hand-over Aircraft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sub-Function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Debt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Complexity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">API Ver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Light / Dark Mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">normal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Splash Screen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Web</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android 12+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Processing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get Current Date / Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move to future provider as stream</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sig-in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Refactor Menu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use-case if user is already signed in (user / club)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Font Size in Widgets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switch to Theme Style with delta Size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Routing to Sign-In</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Go to Sign-in form in case of 401 response</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tab order, skip icon button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skip icon buttons for navigation in form</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Register</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Active Login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auto Login (credential stored in the App)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plane Text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Club Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LogAs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserOrClub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Club</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ListedClub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conditions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AppBar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Settings Icon Top-Right Corner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bottom Panel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Representation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visibility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Register New User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Done</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sign-in User from Sing-in Form</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plain password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sign-in User at App Start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hashed password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sign-in User in On-line mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change User Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password shall not be used by other users</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Password Recover</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change User Avatar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Personal Data Download</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mark user as deleted in DB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Days Impl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sing-in Club from Sign-In Form</t>
-  </si>
-  <si>
-    <t xml:space="preserve">increased</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sign-in Club at App Start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sign-in Club Once switching to On-Line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rename Club</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change Club Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Join Club</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password check</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If Member</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change Club Avatar</t>
-  </si>
-  <si>
     <t xml:space="preserve">Add members to Club</t>
   </si>
   <si>
@@ -449,16 +472,155 @@
   </si>
   <si>
     <t xml:space="preserve">Set roles to members</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Response Codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin Block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SrvUsr Block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Corner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register a new user and a dedicated club</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ok / Conflict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sing-in to the system as user or club</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ok / Unauthorized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CheckUserNameFree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checks if provided user name is free</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChangeUserPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shall be requested by a user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CheckEmailFree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checks if provided email is free</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChangeUserEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RequestUserPasswordReset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GetUserProfile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DeleteUserProfile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CreateClub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a new club by a user request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GetPublicClubs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get the list of public clubs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CheckClubNameFree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checks if provided club name is free</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JoinClub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GetClubDetails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checklist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReadCheckList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ok / Conflict / Unauthorized / NotFound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Previous Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check username free</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CheckUserNameFreeResult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CheckValueValidResponse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IsValueValid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete file after refactor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check email free</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CheckEmailFreeResult</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$-407]dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="[$-407]General"/>
+    <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -500,7 +662,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00A933"/>
-        <bgColor rgb="FF008000"/>
+        <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
     <fill>
@@ -550,7 +712,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -587,23 +749,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -634,7 +784,7 @@
     <cellStyle name="Green" xfId="20"/>
     <cellStyle name="Untitled1" xfId="21"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
     <dxf>
       <font>
         <name val="Arial"/>
@@ -792,6 +942,32 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF006600"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
@@ -804,7 +980,7 @@
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
@@ -861,10 +1037,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -985,9 +1161,15 @@
       <c r="C5" s="2" t="n">
         <v>44920</v>
       </c>
+      <c r="D5" s="2" t="n">
+        <v>45017</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>45047</v>
+      </c>
       <c r="G5" s="9" t="str">
         <f aca="false">IF(ISBLANK(D5),"Open",(IF(ISBLANK($E5),"Processing","Done")))</f>
-        <v>Open</v>
+        <v>Done</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -998,9 +1180,12 @@
       <c r="C6" s="2" t="n">
         <v>44920</v>
       </c>
+      <c r="D6" s="2" t="n">
+        <v>45017</v>
+      </c>
       <c r="G6" s="9" t="str">
         <f aca="false">IF(ISBLANK(D6),"Open",(IF(ISBLANK($E6),"Processing","Done")))</f>
-        <v>Open</v>
+        <v>Processing</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1131,6 +1316,19 @@
       </c>
       <c r="C12" s="2" t="n">
         <v>44920</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1163,490 +1361,652 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="18.99"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="11" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="19.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="2" style="11" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10"/>
-      <c r="B1" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="12" t="s">
+      <c r="B1" s="4" t="s">
         <v>32</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>39</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>39</v>
+        <v>45</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>36</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>52</v>
+        <v>38</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>52</v>
+        <v>39</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>52</v>
+        <v>39</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0"/>
+      <c r="A30" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0"/>
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:E1048576">
+  <conditionalFormatting sqref="B1:F1048576">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"X"</formula>
     </cfRule>
@@ -1676,38 +2036,38 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="23.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="40.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="14" width="11.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="14" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="14" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="40.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="11.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="2" width="11.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="9" width="10.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="10" width="10.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>2</v>
@@ -1728,25 +2088,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="D2" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" s="15"/>
+      <c r="D2" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="12"/>
       <c r="G2" s="2" t="n">
         <v>44920</v>
       </c>
-      <c r="H2" s="16" t="n">
+      <c r="H2" s="13" t="n">
         <v>44921</v>
       </c>
-      <c r="I2" s="16"/>
+      <c r="I2" s="13"/>
       <c r="J2" s="1" t="n">
         <f aca="false">I2-H2</f>
         <v>-44921</v>
@@ -1757,17 +2117,17 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
-        <v>71</v>
+      <c r="A3" s="14" t="s">
+        <v>80</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>70</v>
+        <v>81</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>44920</v>
@@ -1783,20 +2143,20 @@
         <v>0</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="L3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>70</v>
+        <v>83</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>44940</v>
@@ -1806,19 +2166,19 @@
         <v>0</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>70</v>
+        <v>85</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>44920</v>
@@ -1840,16 +2200,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>70</v>
+      <c r="E6" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>44940</v>
@@ -1870,17 +2230,17 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>79</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>70</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>44940</v>
@@ -1895,15 +2255,15 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17"/>
-      <c r="C8" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>70</v>
+      <c r="A8" s="14"/>
+      <c r="C8" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>44940</v>
@@ -1921,16 +2281,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>70</v>
+        <v>91</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>44940</v>
@@ -1945,16 +2305,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>70</v>
+        <v>94</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>44983</v>
@@ -1966,16 +2326,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>70</v>
+        <v>96</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>44983</v>
@@ -2085,133 +2445,133 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>93</v>
+      <c r="A2" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>95</v>
+      <c r="A3" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>93</v>
+      <c r="A5" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>95</v>
+      <c r="A6" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>100</v>
+      <c r="A8" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>99</v>
+      <c r="E9" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H10" s="9" t="s">
-        <v>101</v>
+      <c r="H10" s="10" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2233,38 +2593,38 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="36.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="14" width="11.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="14" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="14" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="36.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="11.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="2" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>2</v>
@@ -2287,22 +2647,22 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15" t="n">
+        <v>114</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>44920</v>
       </c>
-      <c r="J2" s="9"/>
+      <c r="J2" s="10"/>
       <c r="K2" s="9" t="str">
         <f aca="false">IF(ISBLANK(H3),"Open",(IF(ISBLANK($I3),"Processing","Done")))</f>
         <v>Open</v>
@@ -2310,52 +2670,52 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+        <v>116</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
+        <v>117</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+        <v>118</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K1:K1048576">
@@ -2478,38 +2838,38 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="36.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="14" width="11.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="14" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="14" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="36.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="11.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="2" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>2</v>
@@ -2532,13 +2892,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15" t="n">
+        <v>119</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="n">
@@ -2550,84 +2913,100 @@
       <c r="I2" s="2" t="n">
         <v>44972</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9" t="s">
-        <v>111</v>
+      <c r="J2" s="10"/>
+      <c r="K2" s="9" t="str">
+        <f aca="false">IF(ISBLANK(G2),"Open",(IF(ISBLANK($H2),"Processing","Done")))</f>
+        <v>Done</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15" t="n">
+        <v>121</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>44920</v>
       </c>
-      <c r="K3" s="9" t="s">
-        <v>111</v>
+      <c r="K3" s="9" t="str">
+        <f aca="false">IF(ISBLANK(G3),"Open",(IF(ISBLANK($H3),"Processing","Done")))</f>
+        <v>Processing</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15" t="n">
+        <v>123</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>44920</v>
       </c>
-      <c r="K4" s="9" t="s">
-        <v>73</v>
+      <c r="H4" s="2" t="n">
+        <v>45031</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>45046</v>
+      </c>
+      <c r="K4" s="9" t="str">
+        <f aca="false">IF(ISBLANK(G4),"Open",(IF(ISBLANK($H4),"Processing","Done")))</f>
+        <v>Done</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15" t="n">
+        <v>125</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>44920</v>
       </c>
-      <c r="K5" s="9" t="s">
-        <v>73</v>
+      <c r="K5" s="9" t="str">
+        <f aca="false">IF(ISBLANK(G5),"Open",(IF(ISBLANK($H5),"Processing","Done")))</f>
+        <v>Processing</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15" t="n">
+      <c r="D6" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="n">
@@ -2639,22 +3018,23 @@
       <c r="I6" s="2" t="n">
         <v>44985</v>
       </c>
-      <c r="K6" s="9" t="s">
-        <v>111</v>
+      <c r="K6" s="9" t="str">
+        <f aca="false">IF(ISBLANK(G6),"Open",(IF(ISBLANK($H6),"Processing","Done")))</f>
+        <v>Done</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15" t="n">
+        <v>127</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="n">
@@ -2667,19 +3047,19 @@
         <v>44990</v>
       </c>
       <c r="K7" s="9" t="str">
-        <f aca="false">IF(ISBLANK(H8),"Open",(IF(ISBLANK($I8),"Processing","Done")))</f>
+        <f aca="false">IF(ISBLANK(G7),"Open",(IF(ISBLANK($H7),"Processing","Done")))</f>
         <v>Done</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15" t="n">
+        <v>129</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="n">
@@ -2692,54 +3072,54 @@
         <v>44946</v>
       </c>
       <c r="K8" s="9" t="str">
-        <f aca="false">IF(ISBLANK(H9),"Open",(IF(ISBLANK($I9),"Processing","Done")))</f>
-        <v>Open</v>
+        <f aca="false">IF(ISBLANK(G8),"Open",(IF(ISBLANK($H8),"Processing","Done")))</f>
+        <v>Done</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="E9" s="15"/>
+        <v>130</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E9" s="12"/>
       <c r="G9" s="2" t="n">
         <v>44920</v>
       </c>
       <c r="K9" s="9" t="str">
-        <f aca="false">IF(ISBLANK(H10),"Open",(IF(ISBLANK($I10),"Processing","Done")))</f>
-        <v>Open</v>
+        <f aca="false">IF(ISBLANK(G9),"Open",(IF(ISBLANK($H9),"Processing","Done")))</f>
+        <v>Processing</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="E10" s="15"/>
+        <v>132</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E10" s="12"/>
       <c r="G10" s="2" t="n">
         <v>44920</v>
       </c>
       <c r="K10" s="9" t="str">
-        <f aca="false">IF(ISBLANK(H11),"Open",(IF(ISBLANK($I11),"Processing","Done")))</f>
-        <v>Done</v>
+        <f aca="false">IF(ISBLANK(G10),"Open",(IF(ISBLANK($H10),"Processing","Done")))</f>
+        <v>Processing</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="14" t="n">
+        <v>134</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="11" t="n">
         <v>1</v>
       </c>
       <c r="G11" s="2" t="n">
@@ -2751,8 +3131,9 @@
       <c r="I11" s="2" t="n">
         <v>45000</v>
       </c>
-      <c r="K11" s="9" t="s">
-        <v>111</v>
+      <c r="K11" s="9" t="str">
+        <f aca="false">IF(ISBLANK(G11),"Open",(IF(ISBLANK($H11),"Processing","Done")))</f>
+        <v>Done</v>
       </c>
     </row>
   </sheetData>
@@ -2921,34 +3302,34 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="36.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="11.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="14" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="14" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="36.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="11.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="2" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>2</v>
@@ -2960,7 +3341,7 @@
         <v>4</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>6</v>
@@ -2971,31 +3352,37 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="15"/>
+        <v>37</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="12"/>
       <c r="F2" s="2" t="n">
         <v>44835</v>
       </c>
+      <c r="G2" s="2" t="n">
+        <v>44986</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>45000</v>
+      </c>
       <c r="J2" s="9" t="str">
-        <f aca="false">IF(ISBLANK(H6),"Open",(IF(ISBLANK($I6),"Processing","Done")))</f>
-        <v>Open</v>
+        <f aca="false">IF(ISBLANK(G2),"Open",(IF(ISBLANK($H2),"Processing","Done")))</f>
+        <v>Done</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="E3" s="15"/>
+        <v>136</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="12"/>
       <c r="F3" s="2" t="n">
         <v>44835</v>
       </c>
@@ -3005,26 +3392,26 @@
       <c r="H3" s="2" t="n">
         <v>44906</v>
       </c>
-      <c r="I3" s="9" t="n">
+      <c r="I3" s="10" t="n">
         <f aca="false">H3-G3</f>
         <v>71</v>
       </c>
       <c r="J3" s="9" t="str">
-        <f aca="false">IF(ISBLANK(H7),"Open",(IF(ISBLANK($I7),"Processing","Done")))</f>
-        <v>Open</v>
+        <f aca="false">IF(ISBLANK(G3),"Open",(IF(ISBLANK($H3),"Processing","Done")))</f>
+        <v>Done</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="E4" s="15"/>
+        <v>138</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E4" s="12"/>
       <c r="F4" s="2" t="n">
         <v>44835</v>
       </c>
@@ -3035,21 +3422,21 @@
         <v>44906</v>
       </c>
       <c r="J4" s="9" t="str">
-        <f aca="false">IF(ISBLANK(H8),"Open",(IF(ISBLANK($I8),"Processing","Done")))</f>
-        <v>Open</v>
+        <f aca="false">IF(ISBLANK(G4),"Open",(IF(ISBLANK($H4),"Processing","Done")))</f>
+        <v>Done</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="E5" s="15"/>
+        <v>139</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="12"/>
       <c r="F5" s="2" t="n">
         <v>44835</v>
       </c>
@@ -3060,178 +3447,176 @@
         <v>44906</v>
       </c>
       <c r="J5" s="9" t="str">
-        <f aca="false">IF(ISBLANK(H9),"Open",(IF(ISBLANK($I9),"Processing","Done")))</f>
-        <v>Open</v>
+        <f aca="false">IF(ISBLANK(G5),"Open",(IF(ISBLANK($H5),"Processing","Done")))</f>
+        <v>Done</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="15"/>
+        <v>140</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="12"/>
       <c r="F6" s="2" t="n">
         <v>44835</v>
       </c>
       <c r="J6" s="9" t="str">
-        <f aca="false">IF(ISBLANK(H9),"Open",(IF(ISBLANK($I9),"Processing","Done")))</f>
+        <f aca="false">IF(ISBLANK(G6),"Open",(IF(ISBLANK($H6),"Processing","Done")))</f>
         <v>Open</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="15"/>
+        <v>141</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="12"/>
       <c r="F7" s="2" t="n">
         <v>44835</v>
       </c>
       <c r="J7" s="9" t="str">
-        <f aca="false">IF(ISBLANK(H10),"Open",(IF(ISBLANK($I10),"Processing","Done")))</f>
+        <f aca="false">IF(ISBLANK(G7),"Open",(IF(ISBLANK($H7),"Processing","Done")))</f>
         <v>Open</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="15"/>
+        <v>48</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="12"/>
       <c r="F8" s="2" t="n">
         <v>44835</v>
       </c>
+      <c r="G8" s="2" t="n">
+        <v>45031</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>45046</v>
+      </c>
       <c r="J8" s="9" t="str">
-        <f aca="false">IF(ISBLANK(H11),"Open",(IF(ISBLANK($I11),"Processing","Done")))</f>
-        <v>Open</v>
+        <f aca="false">IF(ISBLANK(G8),"Open",(IF(ISBLANK($H8),"Processing","Done")))</f>
+        <v>Done</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" s="15"/>
+        <v>49</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="12"/>
       <c r="F9" s="2" t="n">
         <v>44835</v>
       </c>
       <c r="J9" s="9" t="str">
-        <f aca="false">IF(ISBLANK(H12),"Open",(IF(ISBLANK($I12),"Processing","Done")))</f>
+        <f aca="false">IF(ISBLANK(G9),"Open",(IF(ISBLANK($H9),"Processing","Done")))</f>
         <v>Open</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="15"/>
+        <v>142</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="12"/>
       <c r="F10" s="2" t="n">
         <v>44835</v>
       </c>
       <c r="J10" s="9" t="str">
-        <f aca="false">IF(ISBLANK(H13),"Open",(IF(ISBLANK($I13),"Processing","Done")))</f>
+        <f aca="false">IF(ISBLANK(G10),"Open",(IF(ISBLANK($H10),"Processing","Done")))</f>
         <v>Open</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="12"/>
       <c r="F11" s="2" t="n">
         <v>44835</v>
       </c>
       <c r="J11" s="9" t="str">
-        <f aca="false">IF(ISBLANK(H14),"Open",(IF(ISBLANK($I14),"Processing","Done")))</f>
+        <f aca="false">IF(ISBLANK(G11),"Open",(IF(ISBLANK($H11),"Processing","Done")))</f>
         <v>Open</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>84</v>
+        <v>144</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>44983</v>
       </c>
+      <c r="J12" s="9" t="str">
+        <f aca="false">IF(ISBLANK(G12),"Open",(IF(ISBLANK($H12),"Processing","Done")))</f>
+        <v>Open</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>69</v>
+        <v>145</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>131</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>44983</v>
       </c>
+      <c r="J13" s="9" t="str">
+        <f aca="false">IF(ISBLANK(G13),"Open",(IF(ISBLANK($H13),"Processing","Done")))</f>
+        <v>Open</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>69</v>
+        <v>146</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>44983</v>
       </c>
+      <c r="J14" s="9" t="str">
+        <f aca="false">IF(ISBLANK(G14),"Open",(IF(ISBLANK($H14),"Processing","Done")))</f>
+        <v>Open</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>69</v>
+        <v>147</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>44983</v>
+      </c>
+      <c r="J15" s="9" t="str">
+        <f aca="false">IF(ISBLANK(G15),"Open",(IF(ISBLANK($H15),"Processing","Done")))</f>
+        <v>Open</v>
       </c>
     </row>
   </sheetData>
@@ -3373,4 +3758,454 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="12.68"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D1:H1048576">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+      <formula>"Ok"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+      <formula>"Open"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="18.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="20.38"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
17.07.2023 End of the Day, M1 Started to work on club details
</commit_message>
<xml_diff>
--- a/spec/fs_front_fnctions.xlsx
+++ b/spec/fs_front_fnctions.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="196">
   <si>
     <t xml:space="preserve">PI Nr.</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t xml:space="preserve">AccountManage, AppAction, FSA: club_manager IU, GetClubsRolesActionsResponse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.07.2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">requestedActions as List&lt;String&gt; from App =&gt; Web =&gt; convert into List&lt;AppActions&gt; =&gt; check resolution =&gt; return to App</t>
   </si>
   <si>
     <t xml:space="preserve">Next: implement actions for browsing club (get basic info, get user list, add / remove user etc)</t>
@@ -1037,10 +1043,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1319,7 +1325,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1327,8 +1333,16 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="1" t="s">
+      <c r="A17" s="0" t="s">
         <v>31</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1369,625 +1383,625 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="19.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="19.93"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="2" style="11" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10"/>
       <c r="B1" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2052,22 +2066,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>2</v>
@@ -2090,14 +2104,14 @@
     </row>
     <row r="2" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B2" s="1"/>
       <c r="D2" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="2" t="n">
@@ -2118,16 +2132,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="11" t="s">
         <v>81</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>79</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>44920</v>
@@ -2143,20 +2157,20 @@
         <v>0</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14"/>
       <c r="B4" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>44940</v>
@@ -2166,19 +2180,19 @@
         <v>0</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14"/>
       <c r="B5" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>44920</v>
@@ -2200,16 +2214,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>44940</v>
@@ -2231,16 +2245,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>44940</v>
@@ -2257,13 +2271,13 @@
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="14"/>
       <c r="C8" s="10" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>44940</v>
@@ -2281,16 +2295,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>44940</v>
@@ -2305,16 +2319,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>44983</v>
@@ -2326,16 +2340,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>44983</v>
@@ -2452,126 +2466,126 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E8" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>106</v>
-      </c>
       <c r="H8" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E9" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H9" s="10" t="s">
         <v>110</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H10" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2609,22 +2623,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>2</v>
@@ -2647,13 +2661,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12" t="n">
@@ -2670,10 +2684,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
@@ -2681,7 +2695,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
@@ -2689,7 +2703,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
@@ -2854,22 +2868,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>2</v>
@@ -2892,13 +2906,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12" t="n">
@@ -2921,16 +2935,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="12" t="n">
@@ -2946,16 +2960,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12" t="n">
@@ -2977,13 +2991,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12" t="n">
@@ -2999,11 +3013,11 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12" t="n">
@@ -3025,13 +3039,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12" t="n">
@@ -3053,10 +3067,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12" t="n">
@@ -3078,10 +3092,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E9" s="12"/>
       <c r="G9" s="2" t="n">
@@ -3094,10 +3108,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E10" s="12"/>
       <c r="G10" s="2" t="n">
@@ -3110,13 +3124,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="11" t="n">
@@ -3317,19 +3331,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>2</v>
@@ -3341,7 +3355,7 @@
         <v>4</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>6</v>
@@ -3352,10 +3366,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D2" s="12"/>
       <c r="F2" s="2" t="n">
@@ -3374,13 +3388,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="2" t="n">
@@ -3403,13 +3417,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="2" t="n">
@@ -3428,13 +3442,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>139</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>137</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="2" t="n">
@@ -3453,10 +3467,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D6" s="12"/>
       <c r="F6" s="2" t="n">
@@ -3469,10 +3483,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D7" s="12"/>
       <c r="F7" s="2" t="n">
@@ -3485,10 +3499,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D8" s="12"/>
       <c r="F8" s="2" t="n">
@@ -3507,10 +3521,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D9" s="12"/>
       <c r="F9" s="2" t="n">
@@ -3523,10 +3537,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D10" s="12"/>
       <c r="F10" s="2" t="n">
@@ -3537,15 +3551,15 @@
         <v>Open</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D11" s="12"/>
       <c r="F11" s="2" t="n">
@@ -3558,10 +3572,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>44983</v>
@@ -3573,10 +3587,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>44983</v>
@@ -3586,15 +3600,15 @@
         <v>Open</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>44983</v>
@@ -3606,10 +3620,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>44983</v>
@@ -3782,323 +3796,323 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -4144,13 +4158,13 @@
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="5" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>7</v>
@@ -4161,42 +4175,42 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>191</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>